<commit_message>
Aggregated Metrics Into Excel File
</commit_message>
<xml_diff>
--- a/Metrics/Full sheet .xlsx
+++ b/Metrics/Full sheet .xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>Coverage</t>
   </si>
@@ -57,16 +57,116 @@
   </si>
   <si>
     <t>Project</t>
+  </si>
+  <si>
+    <t>Conditionals Boundary Mutator</t>
+  </si>
+  <si>
+    <t>Increments Mutator</t>
+  </si>
+  <si>
+    <t>Void Method Call Mutator</t>
+  </si>
+  <si>
+    <t>Return Vals Mutator</t>
+  </si>
+  <si>
+    <t>Math Mutator</t>
+  </si>
+  <si>
+    <t>Negate Conditionals Mutator</t>
+  </si>
+  <si>
+    <t>Killed</t>
+  </si>
+  <si>
+    <t>Survived</t>
+  </si>
+  <si>
+    <t>No Coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dagger </t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>JACOCO STATS</t>
+  </si>
+  <si>
+    <t>PIT STATS</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Moshi-Initial</t>
+  </si>
+  <si>
+    <t>Invert Negatives Mutator</t>
+  </si>
+  <si>
+    <t>ScribeJava</t>
+  </si>
+  <si>
+    <t>Scan Classpath</t>
+  </si>
+  <si>
+    <t>Coverage / Dependency Analysis</t>
+  </si>
+  <si>
+    <t>Run Mutation Analysis</t>
+  </si>
+  <si>
+    <t>&lt; 1</t>
+  </si>
+  <si>
+    <t>Build Mutation Tests</t>
+  </si>
+  <si>
+    <t>Dagger</t>
+  </si>
+  <si>
+    <t>Moshi</t>
+  </si>
+  <si>
+    <t>Time(sec)</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Generated 557 mutations Killed 353 (63%)</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Ran 4227 tests (7.59 tests per mutation)</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Generated 1703 mutations Killed 1381 (81%)</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Ran 11605 tests (6.81 tests per mutation)</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Generated 1145 mutations Killed 404 (35%)</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Ran 879 tests (0.77 tests per mutation)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,6 +195,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -119,21 +225,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -421,188 +537,760 @@
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="G2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>0.81399999999999995</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <v>9055</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="2">
         <v>2067</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E3" s="2">
         <v>11122</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2">
+        <v>12</v>
+      </c>
+      <c r="K3" s="2">
+        <f>H3+I3+J3</f>
+        <v>28</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>0.86899999999999999</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <v>5578</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>843</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E4" s="2">
         <v>6421</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" ref="K4:K8" si="0">H4+I4+J4</f>
+        <v>6</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>0.73599999999999999</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="2">
         <v>3462</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D5" s="2">
         <v>1239</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E5" s="2">
         <v>4701</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="2">
+        <v>63</v>
+      </c>
+      <c r="I5" s="2">
+        <v>13</v>
+      </c>
+      <c r="J5">
+        <v>25</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>91</v>
+      </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>41</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <v>0.59299999999999997</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="2">
         <v>7682</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D7" s="2">
         <v>5266</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E7" s="2">
         <v>12948</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2">
+        <v>28</v>
+      </c>
+      <c r="I7" s="2">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>52</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>0.49199999999999999</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C8" s="2">
         <v>4402</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D8" s="2">
         <v>4542</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="2">
         <v>8944</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="2">
+        <v>155</v>
+      </c>
+      <c r="I8" s="2">
+        <v>12</v>
+      </c>
+      <c r="J8">
+        <v>31</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="0"/>
+        <v>198</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <v>0.81899999999999995</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="2">
         <v>3280</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>724</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="2">
         <v>4004</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="2">
+        <f>SUM(H3:H8)</f>
+        <v>353</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" ref="I9:K9" si="1">SUM(I3:I8)</f>
+        <v>41</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>163</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="1"/>
+        <v>557</v>
+      </c>
+      <c r="L9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9">
+        <f>SUM(M5:M8)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <v>0.89700000000000002</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
         <v>35505</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="2">
         <v>4059</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E11" s="2">
         <v>39564</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="G11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>0.872</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C12" s="2">
         <v>12486</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <v>1837</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="2">
         <v>14323</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="2">
+        <v>54</v>
+      </c>
+      <c r="I12" s="2">
+        <v>13</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
+        <f>H12+I12+J12</f>
+        <v>68</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>0.91200000000000003</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C13" s="2">
         <v>23019</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D13" s="2">
         <v>2222</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E13" s="2">
         <v>25241</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>28</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" ref="K13:K18" si="2">H13+I13+J13</f>
+        <v>29</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="2">
+        <v>128</v>
+      </c>
+      <c r="I14" s="2">
+        <v>28</v>
+      </c>
+      <c r="J14">
+        <v>17</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="2"/>
+        <v>173</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>319</v>
+      </c>
+      <c r="I15">
+        <v>65</v>
+      </c>
+      <c r="J15">
+        <v>64</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="2"/>
+        <v>448</v>
+      </c>
+      <c r="L15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="2">
+        <v>196</v>
+      </c>
+      <c r="I16" s="2">
+        <v>52</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="L16" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="2">
+        <v>654</v>
+      </c>
+      <c r="I17" s="2">
+        <v>40</v>
+      </c>
+      <c r="J17">
+        <v>39</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="2"/>
+        <v>733</v>
+      </c>
+      <c r="L17" t="s">
+        <v>31</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="6">
+        <v>2</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="L18" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18" s="2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="2">
+        <f>SUM(H12:H18)</f>
+        <v>1381</v>
+      </c>
+      <c r="I19" s="2">
+        <f>SUM(I12:I18)</f>
+        <v>199</v>
+      </c>
+      <c r="J19" s="2">
+        <f>SUM(J12:J18)</f>
+        <v>123</v>
+      </c>
+      <c r="K19" s="2">
+        <f>SUM(K12:K18)</f>
+        <v>1703</v>
+      </c>
+      <c r="L19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19">
+        <f>SUM(M15:M18)</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="2">
+        <v>12</v>
+      </c>
+      <c r="I22" s="2">
+        <v>14</v>
+      </c>
+      <c r="J22" s="2">
+        <v>20</v>
+      </c>
+      <c r="K22" s="2">
+        <f>H22+I22+J22</f>
+        <v>46</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23">
+        <v>20</v>
+      </c>
+      <c r="I23">
+        <v>6</v>
+      </c>
+      <c r="J23">
+        <v>27</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" ref="K23:K27" si="3">H23+I23+J23</f>
+        <v>53</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="2">
+        <v>51</v>
+      </c>
+      <c r="I24" s="2">
+        <v>16</v>
+      </c>
+      <c r="J24">
+        <v>165</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="L24" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25">
+        <v>143</v>
+      </c>
+      <c r="I25">
+        <v>8</v>
+      </c>
+      <c r="J25">
+        <v>200</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="3"/>
+        <v>351</v>
+      </c>
+      <c r="L25" t="s">
+        <v>28</v>
+      </c>
+      <c r="M25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="2">
+        <v>50</v>
+      </c>
+      <c r="I26" s="2">
+        <v>20</v>
+      </c>
+      <c r="J26">
+        <v>101</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="3"/>
+        <v>171</v>
+      </c>
+      <c r="L26" t="s">
+        <v>31</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="2">
+        <v>128</v>
+      </c>
+      <c r="I27" s="2">
+        <v>36</v>
+      </c>
+      <c r="J27">
+        <v>128</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="3"/>
+        <v>292</v>
+      </c>
+      <c r="L27" t="s">
+        <v>29</v>
+      </c>
+      <c r="M27" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="2">
+        <f>SUM(H22:H27)</f>
+        <v>404</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" ref="I28" si="4">SUM(I22:I27)</f>
+        <v>100</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" ref="J28" si="5">SUM(J22:J27)</f>
+        <v>641</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" ref="K28" si="6">SUM(K22:K27)</f>
+        <v>1145</v>
+      </c>
+      <c r="L28" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28">
+        <f>SUM(M24:M27)</f>
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mutant Killer Suite Up and Running
Killed 8 mutants in 2 classes
</commit_message>
<xml_diff>
--- a/Metrics/Full sheet .xlsx
+++ b/Metrics/Full sheet .xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
   <si>
     <t>Coverage</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>&gt;&gt; Ran 879 tests (0.77 tests per mutation)</t>
+  </si>
+  <si>
+    <t>Includes Other Outcomes</t>
   </si>
 </sst>
 </file>
@@ -527,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,6 +541,7 @@
     <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -547,6 +551,9 @@
       </c>
       <c r="G1" t="s">
         <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>